<commit_message>
#0000 Documentation: Update of content
</commit_message>
<xml_diff>
--- a/seanox_ai_nlp/units/units.xlsx
+++ b/seanox_ai_nlp/units/units.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="217">
   <si>
     <t xml:space="preserve">Unit</t>
   </si>
@@ -49,16 +49,13 @@
     <t xml:space="preserve">Common Units</t>
   </si>
   <si>
-    <t xml:space="preserve">Informal Phrase</t>
+    <t xml:space="preserve">Common Phrase</t>
   </si>
   <si>
     <t xml:space="preserve">Informal Prefix</t>
   </si>
   <si>
     <t xml:space="preserve">Informal Exponents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Informal</t>
   </si>
   <si>
     <t xml:space="preserve">(Arc) Minute</t>
@@ -1188,11 +1185,11 @@
   <dimension ref="A1:XFD128"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C74" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A74" activeCellId="0" sqref="A74"/>
+      <selection pane="bottomRight" activeCell="C74" activeCellId="0" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9140625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1217,7 +1214,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="8.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="12.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="8.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="15.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="14.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="18.41"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16378" min="24" style="1" width="10.91"/>
@@ -1250,7 +1247,7 @@
       </c>
       <c r="T1" s="9" t="str">
         <f aca="false">IF(LEN(_xlfn.CONCAT(T3:T112)) &gt; 0,LEFT(_xlfn.CONCAT(T3:T112),LEN(_xlfn.CONCAT(T3:T112)) -1),"")</f>
-        <v>′|″|″|a|a|a|Ah|atm|Atü|bar|bbl|d|dam|dB|db(A)|db(C)|db(G)|db(Z)|dpt|dz|Dz|ft|gal|ha|hl|hp|in|kn|kt|kt|l|L|lb|lj|ls|mel|mi|min|Np|º|oz|oz.|p|pc|PS|rad|rm|sone|sq.ft.|sq.in.|sq.mile|sq.yd.|sq. ft.|sq. in.|sq. mile|sq. yd.|sq ft|sq in|sq mile|sq yd|St|t|tex|u|v|VA|Var|Wh|yd|Z|ρ|ω</v>
+        <v>′|″|″|a|a|a|Ah|atm|Atü|bar|bbl|d|dam|dB|db(A)|db(C)|db(G)|db(Z)|dpt|dz|Dz|ft|gal|ha|hl|hp|in|kn|kt|kt|l|L|lb|lj|ls|mel|mi|min|Np|º|oz|oz.|p|pc|PS|rad|rm|sone|St|t|tex|u|v|VA|Var|Wh|yd|Z|ρ|ω</v>
       </c>
       <c r="U1" s="10" t="str">
         <f aca="false">IF(LEN(_xlfn.CONCAT(U3:U112)) &gt; 0,LEFT(_xlfn.CONCAT(U3:U112),LEN(_xlfn.CONCAT(U3:U112)) -1),"")</f>
@@ -1324,7 +1321,7 @@
         <v>8</v>
       </c>
       <c r="U2" s="13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="V2" s="13" t="s">
         <v>10</v>
@@ -1332,8 +1329,8 @@
       <c r="W2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="XEY2" s="0"/>
-      <c r="XEZ2" s="0"/>
+      <c r="XEY2" s="15"/>
+      <c r="XEZ2" s="15"/>
       <c r="XFA2" s="15"/>
       <c r="XFB2" s="15"/>
       <c r="XFC2" s="15"/>
@@ -1341,10 +1338,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>14</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
@@ -1402,10 +1399,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="17" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>16</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
@@ -1463,10 +1460,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="16"/>
@@ -1524,10 +1521,10 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>18</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>19</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
@@ -1585,24 +1582,24 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="17" t="s">
-        <v>21</v>
-      </c>
       <c r="C7" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
       <c r="F7" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" s="16" t="str">
         <f aca="false">IF(G7="","x","")</f>
@@ -1654,18 +1651,18 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
       <c r="E8" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
@@ -1675,10 +1672,10 @@
       </c>
       <c r="J8" s="16"/>
       <c r="K8" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N8" s="1" t="str">
         <f aca="false">IF(C8&lt;&gt;"",$B8&amp;"|","")</f>
@@ -1723,10 +1720,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
@@ -1784,21 +1781,21 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>25</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>26</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H10" s="16"/>
       <c r="I10" s="16" t="str">
@@ -1851,16 +1848,16 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G11" s="16"/>
       <c r="I11" s="16" t="str">
@@ -1910,10 +1907,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>29</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>30</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
@@ -1971,10 +1968,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>31</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>32</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
@@ -2032,21 +2029,21 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H14" s="16"/>
       <c r="I14" s="16" t="str">
@@ -2099,21 +2096,21 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>34</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>35</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H15" s="16"/>
       <c r="I15" s="16" t="str">
@@ -2166,21 +2163,21 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>36</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>37</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="16" t="str">
@@ -2233,18 +2230,18 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="17" t="s">
         <v>38</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>39</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
       <c r="E17" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G17" s="16"/>
       <c r="H17" s="16"/>
@@ -2298,10 +2295,10 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="17" t="s">
         <v>40</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>41</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -2359,24 +2356,24 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="17" t="s">
         <v>42</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>43</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E19" s="16"/>
       <c r="F19" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I19" s="16" t="str">
         <f aca="false">IF(G19="","x","")</f>
@@ -2428,24 +2425,24 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>44</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>45</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E20" s="16"/>
       <c r="F20" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I20" s="16" t="str">
         <f aca="false">IF(G20="","x","")</f>
@@ -2497,24 +2494,24 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>47</v>
-      </c>
       <c r="C21" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
       <c r="F21" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I21" s="16" t="str">
         <f aca="false">IF(G21="","x","")</f>
@@ -2566,21 +2563,21 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="17" t="s">
         <v>48</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>49</v>
       </c>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
       <c r="E22" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H22" s="16"/>
       <c r="I22" s="16" t="str">
@@ -2633,18 +2630,18 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>50</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>51</v>
       </c>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
       <c r="E23" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G23" s="16"/>
       <c r="H23" s="16"/>
@@ -2698,19 +2695,19 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="E24" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I24" s="16" t="str">
         <f aca="false">IF(G24="","x","")</f>
@@ -2759,10 +2756,10 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="17" t="s">
         <v>54</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>55</v>
       </c>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
@@ -2820,18 +2817,18 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="17" t="s">
         <v>56</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>57</v>
       </c>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
       <c r="E26" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G26" s="16"/>
       <c r="H26" s="16"/>
@@ -2885,16 +2882,16 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="E27" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G27" s="16"/>
       <c r="I27" s="16" t="str">
@@ -2944,16 +2941,16 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="E28" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G28" s="16"/>
       <c r="I28" s="16" t="str">
@@ -3003,16 +3000,16 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="E29" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G29" s="16"/>
       <c r="I29" s="16" t="str">
@@ -3062,16 +3059,16 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="E30" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G30" s="16"/>
       <c r="I30" s="16" t="str">
@@ -3121,18 +3118,18 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="17" t="s">
         <v>66</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>67</v>
       </c>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
       <c r="E31" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G31" s="16"/>
       <c r="H31" s="16"/>
@@ -3186,10 +3183,10 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="17" t="s">
         <v>68</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>69</v>
       </c>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
@@ -3247,10 +3244,10 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="17" t="s">
         <v>70</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>71</v>
       </c>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
@@ -3308,19 +3305,19 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="E34" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G34" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I34" s="16" t="str">
         <f aca="false">IF(G34="","x","")</f>
@@ -3369,24 +3366,24 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="17" t="s">
         <v>74</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>75</v>
       </c>
       <c r="C35" s="16"/>
       <c r="D35" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E35" s="16"/>
       <c r="F35" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G35" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H35" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I35" s="16" t="str">
         <f aca="false">IF(G35="","x","")</f>
@@ -3438,10 +3435,10 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="17" t="s">
         <v>76</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>77</v>
       </c>
       <c r="C36" s="16"/>
       <c r="D36" s="16"/>
@@ -3499,21 +3496,21 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B37" s="17" t="s">
-        <v>79</v>
-      </c>
       <c r="C37" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="16"/>
       <c r="F37" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H37" s="16"/>
       <c r="I37" s="16" t="str">
@@ -3566,10 +3563,10 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="17" t="s">
         <v>80</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>81</v>
       </c>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
@@ -3627,24 +3624,24 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="17" t="s">
         <v>82</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>83</v>
       </c>
       <c r="C39" s="16"/>
       <c r="D39" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E39" s="16"/>
       <c r="F39" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G39" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I39" s="16" t="str">
         <f aca="false">IF(G39="","x","")</f>
@@ -3696,24 +3693,24 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" s="17" t="s">
         <v>84</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>85</v>
       </c>
       <c r="C40" s="16"/>
       <c r="D40" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E40" s="16"/>
       <c r="F40" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G40" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I40" s="16" t="str">
         <f aca="false">IF(G40="","x","")</f>
@@ -3765,21 +3762,21 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="17" t="s">
         <v>86</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>87</v>
       </c>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
       <c r="E41" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G41" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H41" s="16"/>
       <c r="I41" s="16" t="str">
@@ -3832,18 +3829,18 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" s="17" t="s">
         <v>88</v>
-      </c>
-      <c r="B42" s="17" t="s">
-        <v>89</v>
       </c>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
       <c r="E42" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F42" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G42" s="16"/>
       <c r="H42" s="16"/>
@@ -3853,10 +3850,10 @@
       </c>
       <c r="J42" s="16"/>
       <c r="K42" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L42" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N42" s="1" t="str">
         <f aca="false">IF(C42&lt;&gt;"",$B42&amp;"|","")</f>
@@ -3901,10 +3898,10 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B43" s="17" t="s">
         <v>90</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>91</v>
       </c>
       <c r="C43" s="16"/>
       <c r="D43" s="16"/>
@@ -3962,10 +3959,10 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" s="17" t="s">
         <v>92</v>
-      </c>
-      <c r="B44" s="17" t="s">
-        <v>93</v>
       </c>
       <c r="C44" s="16"/>
       <c r="D44" s="16"/>
@@ -4023,24 +4020,24 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45" s="17" t="s">
         <v>94</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>95</v>
       </c>
       <c r="C45" s="16"/>
       <c r="D45" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E45" s="16"/>
       <c r="F45" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G45" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H45" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I45" s="16" t="str">
         <f aca="false">IF(G45="","x","")</f>
@@ -4092,10 +4089,10 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46" s="17" t="s">
         <v>96</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>97</v>
       </c>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
@@ -4153,24 +4150,24 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" s="17" t="s">
         <v>98</v>
-      </c>
-      <c r="B47" s="17" t="s">
-        <v>99</v>
       </c>
       <c r="C47" s="16"/>
       <c r="D47" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E47" s="16"/>
       <c r="F47" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G47" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I47" s="16" t="str">
         <f aca="false">IF(G47="","x","")</f>
@@ -4222,24 +4219,24 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B48" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="B48" s="17" t="s">
-        <v>101</v>
-      </c>
       <c r="C48" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D48" s="16"/>
       <c r="E48" s="16"/>
       <c r="F48" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G48" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I48" s="16" t="str">
         <f aca="false">IF(G48="","x","")</f>
@@ -4291,24 +4288,24 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49" s="17" t="s">
         <v>102</v>
-      </c>
-      <c r="B49" s="17" t="s">
-        <v>103</v>
       </c>
       <c r="C49" s="16"/>
       <c r="D49" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E49" s="16"/>
       <c r="F49" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G49" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H49" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I49" s="16" t="str">
         <f aca="false">IF(G49="","x","")</f>
@@ -4360,18 +4357,18 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" s="17" t="s">
         <v>104</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>105</v>
       </c>
       <c r="C50" s="16"/>
       <c r="D50" s="16"/>
       <c r="E50" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F50" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G50" s="16"/>
       <c r="H50" s="16"/>
@@ -4425,10 +4422,10 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B51" s="17" t="s">
         <v>106</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>107</v>
       </c>
       <c r="C51" s="16"/>
       <c r="D51" s="16"/>
@@ -4486,18 +4483,18 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
       <c r="E52" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F52" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G52" s="16"/>
       <c r="H52" s="16"/>
@@ -4551,18 +4548,18 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B53" s="17" t="s">
         <v>108</v>
-      </c>
-      <c r="B53" s="17" t="s">
-        <v>109</v>
       </c>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
       <c r="E53" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F53" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G53" s="16"/>
       <c r="H53" s="16"/>
@@ -4616,18 +4613,18 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C54" s="16"/>
       <c r="D54" s="16"/>
       <c r="E54" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G54" s="16"/>
       <c r="H54" s="16"/>
@@ -4681,10 +4678,10 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B55" s="17" t="s">
         <v>111</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>112</v>
       </c>
       <c r="C55" s="16"/>
       <c r="D55" s="16"/>
@@ -4742,10 +4739,10 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B56" s="17" t="s">
         <v>113</v>
-      </c>
-      <c r="B56" s="17" t="s">
-        <v>114</v>
       </c>
       <c r="C56" s="16"/>
       <c r="D56" s="16"/>
@@ -4803,24 +4800,24 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B57" s="17" t="s">
         <v>115</v>
-      </c>
-      <c r="B57" s="17" t="s">
-        <v>116</v>
       </c>
       <c r="C57" s="16"/>
       <c r="D57" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E57" s="16"/>
       <c r="F57" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G57" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H57" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I57" s="16" t="str">
         <f aca="false">IF(G57="","x","")</f>
@@ -4872,10 +4869,10 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" s="17" t="s">
         <v>117</v>
-      </c>
-      <c r="B58" s="17" t="s">
-        <v>118</v>
       </c>
       <c r="C58" s="16"/>
       <c r="D58" s="16"/>
@@ -4933,24 +4930,24 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59" s="17" t="s">
         <v>119</v>
-      </c>
-      <c r="B59" s="17" t="s">
-        <v>120</v>
       </c>
       <c r="C59" s="16"/>
       <c r="D59" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E59" s="16"/>
       <c r="F59" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G59" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H59" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I59" s="16" t="str">
         <f aca="false">IF(G59="","x","")</f>
@@ -5002,24 +4999,24 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="B60" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B60" s="17" t="s">
-        <v>122</v>
-      </c>
       <c r="C60" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D60" s="16"/>
       <c r="E60" s="16"/>
       <c r="F60" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G60" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H60" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I60" s="16" t="str">
         <f aca="false">IF(G60="","x","")</f>
@@ -5027,10 +5024,10 @@
       </c>
       <c r="J60" s="16"/>
       <c r="K60" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L60" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N60" s="1" t="str">
         <f aca="false">IF(C60&lt;&gt;"",$B60&amp;"|","")</f>
@@ -5075,18 +5072,18 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B61" s="17" t="s">
         <v>123</v>
-      </c>
-      <c r="B61" s="17" t="s">
-        <v>124</v>
       </c>
       <c r="C61" s="16"/>
       <c r="D61" s="16"/>
       <c r="E61" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F61" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G61" s="16"/>
       <c r="H61" s="16"/>
@@ -5140,10 +5137,10 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B62" s="17" t="s">
         <v>125</v>
-      </c>
-      <c r="B62" s="17" t="s">
-        <v>126</v>
       </c>
       <c r="C62" s="16"/>
       <c r="D62" s="16"/>
@@ -5157,10 +5154,10 @@
       </c>
       <c r="J62" s="16"/>
       <c r="K62" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L62" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N62" s="1" t="str">
         <f aca="false">IF(C62&lt;&gt;"",$B62&amp;"|","")</f>
@@ -5205,18 +5202,18 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" s="17" t="s">
         <v>127</v>
-      </c>
-      <c r="B63" s="17" t="s">
-        <v>128</v>
       </c>
       <c r="C63" s="16"/>
       <c r="D63" s="16"/>
       <c r="E63" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F63" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G63" s="16"/>
       <c r="H63" s="16"/>
@@ -5270,24 +5267,24 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="B64" s="17" t="s">
-        <v>130</v>
-      </c>
       <c r="C64" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D64" s="16"/>
       <c r="E64" s="16"/>
       <c r="F64" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G64" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H64" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I64" s="16" t="str">
         <f aca="false">IF(G64="","x","")</f>
@@ -5339,21 +5336,21 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B65" s="17" t="s">
         <v>131</v>
-      </c>
-      <c r="B65" s="17" t="s">
-        <v>132</v>
       </c>
       <c r="C65" s="16"/>
       <c r="D65" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E65" s="16"/>
       <c r="F65" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G65" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H65" s="16"/>
       <c r="I65" s="16" t="str">
@@ -5406,18 +5403,18 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B66" s="17" t="s">
         <v>133</v>
-      </c>
-      <c r="B66" s="17" t="s">
-        <v>134</v>
       </c>
       <c r="C66" s="16"/>
       <c r="D66" s="16"/>
       <c r="E66" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F66" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G66" s="16"/>
       <c r="H66" s="16"/>
@@ -5471,10 +5468,10 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B67" s="17" t="s">
         <v>135</v>
-      </c>
-      <c r="B67" s="17" t="s">
-        <v>136</v>
       </c>
       <c r="C67" s="16"/>
       <c r="D67" s="16"/>
@@ -5532,21 +5529,21 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B68" s="17" t="s">
         <v>137</v>
-      </c>
-      <c r="B68" s="17" t="s">
-        <v>138</v>
       </c>
       <c r="C68" s="16"/>
       <c r="D68" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E68" s="16"/>
       <c r="F68" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G68" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H68" s="16"/>
       <c r="I68" s="16" t="str">
@@ -5599,10 +5596,10 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B69" s="17" t="s">
         <v>139</v>
-      </c>
-      <c r="B69" s="17" t="s">
-        <v>140</v>
       </c>
       <c r="C69" s="16"/>
       <c r="D69" s="16"/>
@@ -5660,10 +5657,10 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C70" s="16"/>
       <c r="D70" s="16"/>
@@ -5721,21 +5718,21 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B71" s="17" t="s">
         <v>142</v>
-      </c>
-      <c r="B71" s="17" t="s">
-        <v>143</v>
       </c>
       <c r="C71" s="16"/>
       <c r="D71" s="16"/>
       <c r="E71" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F71" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G71" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H71" s="16"/>
       <c r="I71" s="16" t="str">
@@ -5788,10 +5785,10 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="B72" s="17" t="s">
         <v>144</v>
-      </c>
-      <c r="B72" s="17" t="s">
-        <v>145</v>
       </c>
       <c r="C72" s="16"/>
       <c r="D72" s="16"/>
@@ -5849,24 +5846,24 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B73" s="17" t="s">
         <v>146</v>
-      </c>
-      <c r="B73" s="17" t="s">
-        <v>147</v>
       </c>
       <c r="C73" s="16"/>
       <c r="D73" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E73" s="16"/>
       <c r="F73" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G73" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H73" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I73" s="16" t="str">
         <f aca="false">IF(G73="","x","")</f>
@@ -5918,10 +5915,10 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B74" s="17" t="s">
         <v>148</v>
-      </c>
-      <c r="B74" s="17" t="s">
-        <v>149</v>
       </c>
       <c r="C74" s="16"/>
       <c r="D74" s="16"/>
@@ -5979,18 +5976,18 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="B75" s="17" t="s">
         <v>150</v>
-      </c>
-      <c r="B75" s="17" t="s">
-        <v>151</v>
       </c>
       <c r="C75" s="16"/>
       <c r="D75" s="16"/>
       <c r="E75" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F75" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G75" s="16"/>
       <c r="H75" s="16"/>
@@ -6044,21 +6041,21 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="B76" s="17" t="s">
         <v>152</v>
-      </c>
-      <c r="B76" s="17" t="s">
-        <v>153</v>
       </c>
       <c r="C76" s="16"/>
       <c r="D76" s="16"/>
       <c r="E76" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F76" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G76" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H76" s="16"/>
       <c r="I76" s="16" t="str">
@@ -6111,18 +6108,18 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="B77" s="17" t="s">
         <v>154</v>
-      </c>
-      <c r="B77" s="17" t="s">
-        <v>155</v>
       </c>
       <c r="C77" s="16"/>
       <c r="D77" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E77" s="16"/>
       <c r="F77" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G77" s="16"/>
       <c r="H77" s="16"/>
@@ -6176,10 +6173,10 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="B78" s="17" t="s">
         <v>156</v>
-      </c>
-      <c r="B78" s="17" t="s">
-        <v>157</v>
       </c>
       <c r="C78" s="16"/>
       <c r="D78" s="16"/>
@@ -6237,24 +6234,24 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B79" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="B79" s="17" t="s">
-        <v>159</v>
-      </c>
       <c r="C79" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D79" s="16"/>
       <c r="E79" s="16"/>
       <c r="F79" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G79" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H79" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I79" s="16" t="str">
         <f aca="false">IF(G79="","x","")</f>
@@ -6306,24 +6303,24 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="B80" s="17" t="s">
         <v>160</v>
-      </c>
-      <c r="B80" s="17" t="s">
-        <v>161</v>
       </c>
       <c r="C80" s="16"/>
       <c r="D80" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E80" s="16"/>
       <c r="F80" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G80" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H80" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I80" s="16" t="str">
         <f aca="false">IF(G80="","x","")</f>
@@ -6375,18 +6372,18 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B81" s="17" t="s">
         <v>162</v>
-      </c>
-      <c r="B81" s="17" t="s">
-        <v>163</v>
       </c>
       <c r="C81" s="16"/>
       <c r="D81" s="16"/>
       <c r="E81" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F81" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G81" s="16"/>
       <c r="H81" s="16"/>
@@ -6440,10 +6437,10 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="B82" s="17" t="s">
         <v>164</v>
-      </c>
-      <c r="B82" s="17" t="s">
-        <v>165</v>
       </c>
       <c r="C82" s="16"/>
       <c r="D82" s="16"/>
@@ -6451,10 +6448,7 @@
       <c r="F82" s="16"/>
       <c r="G82" s="16"/>
       <c r="H82" s="16"/>
-      <c r="I82" s="16" t="str">
-        <f aca="false">IF(G82="","x","")</f>
-        <v>x</v>
-      </c>
+      <c r="I82" s="16"/>
       <c r="J82" s="16" t="str">
         <f aca="false">IF(H82="","x","")</f>
         <v>x</v>
@@ -6487,7 +6481,7 @@
       </c>
       <c r="T82" s="1" t="str">
         <f aca="false">IF(I82&lt;&gt;"",$B82&amp;"|","")</f>
-        <v>sq.ft.|</v>
+        <v/>
       </c>
       <c r="U82" s="1" t="str">
         <f aca="false">IF(J82&lt;&gt;"",$B82&amp;"|","")</f>
@@ -6504,10 +6498,10 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B83" s="17" t="s">
         <v>166</v>
-      </c>
-      <c r="B83" s="17" t="s">
-        <v>167</v>
       </c>
       <c r="C83" s="16"/>
       <c r="D83" s="16"/>
@@ -6515,10 +6509,7 @@
       <c r="F83" s="16"/>
       <c r="G83" s="16"/>
       <c r="H83" s="16"/>
-      <c r="I83" s="16" t="str">
-        <f aca="false">IF(G83="","x","")</f>
-        <v>x</v>
-      </c>
+      <c r="I83" s="16"/>
       <c r="J83" s="16" t="str">
         <f aca="false">IF(H83="","x","")</f>
         <v>x</v>
@@ -6551,7 +6542,7 @@
       </c>
       <c r="T83" s="1" t="str">
         <f aca="false">IF(I83&lt;&gt;"",$B83&amp;"|","")</f>
-        <v>sq.in.|</v>
+        <v/>
       </c>
       <c r="U83" s="1" t="str">
         <f aca="false">IF(J83&lt;&gt;"",$B83&amp;"|","")</f>
@@ -6568,10 +6559,10 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="B84" s="17" t="s">
         <v>168</v>
-      </c>
-      <c r="B84" s="17" t="s">
-        <v>169</v>
       </c>
       <c r="C84" s="16"/>
       <c r="D84" s="16"/>
@@ -6579,10 +6570,7 @@
       <c r="F84" s="16"/>
       <c r="G84" s="16"/>
       <c r="H84" s="16"/>
-      <c r="I84" s="16" t="str">
-        <f aca="false">IF(G84="","x","")</f>
-        <v>x</v>
-      </c>
+      <c r="I84" s="16"/>
       <c r="J84" s="16" t="str">
         <f aca="false">IF(H84="","x","")</f>
         <v>x</v>
@@ -6615,7 +6603,7 @@
       </c>
       <c r="T84" s="1" t="str">
         <f aca="false">IF(I84&lt;&gt;"",$B84&amp;"|","")</f>
-        <v>sq.mile|</v>
+        <v/>
       </c>
       <c r="U84" s="1" t="str">
         <f aca="false">IF(J84&lt;&gt;"",$B84&amp;"|","")</f>
@@ -6632,10 +6620,10 @@
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="B85" s="17" t="s">
         <v>170</v>
-      </c>
-      <c r="B85" s="17" t="s">
-        <v>171</v>
       </c>
       <c r="C85" s="16"/>
       <c r="D85" s="16"/>
@@ -6643,10 +6631,7 @@
       <c r="F85" s="16"/>
       <c r="G85" s="16"/>
       <c r="H85" s="16"/>
-      <c r="I85" s="16" t="str">
-        <f aca="false">IF(G85="","x","")</f>
-        <v>x</v>
-      </c>
+      <c r="I85" s="16"/>
       <c r="J85" s="16" t="str">
         <f aca="false">IF(H85="","x","")</f>
         <v>x</v>
@@ -6679,7 +6664,7 @@
       </c>
       <c r="T85" s="1" t="str">
         <f aca="false">IF(I85&lt;&gt;"",$B85&amp;"|","")</f>
-        <v>sq.yd.|</v>
+        <v/>
       </c>
       <c r="U85" s="1" t="str">
         <f aca="false">IF(J85&lt;&gt;"",$B85&amp;"|","")</f>
@@ -6696,10 +6681,10 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B86" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C86" s="16"/>
       <c r="D86" s="16"/>
@@ -6707,10 +6692,7 @@
       <c r="F86" s="16"/>
       <c r="G86" s="16"/>
       <c r="H86" s="16"/>
-      <c r="I86" s="16" t="str">
-        <f aca="false">IF(G86="","x","")</f>
-        <v>x</v>
-      </c>
+      <c r="I86" s="16"/>
       <c r="J86" s="16" t="str">
         <f aca="false">IF(H86="","x","")</f>
         <v>x</v>
@@ -6743,7 +6725,7 @@
       </c>
       <c r="T86" s="1" t="str">
         <f aca="false">IF(I86&lt;&gt;"",$B86&amp;"|","")</f>
-        <v>sq. ft.|</v>
+        <v/>
       </c>
       <c r="U86" s="1" t="str">
         <f aca="false">IF(J86&lt;&gt;"",$B86&amp;"|","")</f>
@@ -6760,10 +6742,10 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B87" s="17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C87" s="16"/>
       <c r="D87" s="16"/>
@@ -6771,10 +6753,7 @@
       <c r="F87" s="16"/>
       <c r="G87" s="16"/>
       <c r="H87" s="16"/>
-      <c r="I87" s="16" t="str">
-        <f aca="false">IF(G87="","x","")</f>
-        <v>x</v>
-      </c>
+      <c r="I87" s="16"/>
       <c r="J87" s="16" t="str">
         <f aca="false">IF(H87="","x","")</f>
         <v>x</v>
@@ -6807,7 +6786,7 @@
       </c>
       <c r="T87" s="1" t="str">
         <f aca="false">IF(I87&lt;&gt;"",$B87&amp;"|","")</f>
-        <v>sq. in.|</v>
+        <v/>
       </c>
       <c r="U87" s="1" t="str">
         <f aca="false">IF(J87&lt;&gt;"",$B87&amp;"|","")</f>
@@ -6824,10 +6803,10 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B88" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C88" s="16"/>
       <c r="D88" s="16"/>
@@ -6835,10 +6814,7 @@
       <c r="F88" s="16"/>
       <c r="G88" s="16"/>
       <c r="H88" s="16"/>
-      <c r="I88" s="16" t="str">
-        <f aca="false">IF(G88="","x","")</f>
-        <v>x</v>
-      </c>
+      <c r="I88" s="16"/>
       <c r="J88" s="16" t="str">
         <f aca="false">IF(H88="","x","")</f>
         <v>x</v>
@@ -6871,7 +6847,7 @@
       </c>
       <c r="T88" s="1" t="str">
         <f aca="false">IF(I88&lt;&gt;"",$B88&amp;"|","")</f>
-        <v>sq. mile|</v>
+        <v/>
       </c>
       <c r="U88" s="1" t="str">
         <f aca="false">IF(J88&lt;&gt;"",$B88&amp;"|","")</f>
@@ -6888,10 +6864,10 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B89" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C89" s="16"/>
       <c r="D89" s="16"/>
@@ -6899,10 +6875,7 @@
       <c r="F89" s="16"/>
       <c r="G89" s="16"/>
       <c r="H89" s="16"/>
-      <c r="I89" s="16" t="str">
-        <f aca="false">IF(G89="","x","")</f>
-        <v>x</v>
-      </c>
+      <c r="I89" s="16"/>
       <c r="J89" s="16" t="str">
         <f aca="false">IF(H89="","x","")</f>
         <v>x</v>
@@ -6935,7 +6908,7 @@
       </c>
       <c r="T89" s="1" t="str">
         <f aca="false">IF(I89&lt;&gt;"",$B89&amp;"|","")</f>
-        <v>sq. yd.|</v>
+        <v/>
       </c>
       <c r="U89" s="1" t="str">
         <f aca="false">IF(J89&lt;&gt;"",$B89&amp;"|","")</f>
@@ -6952,10 +6925,10 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B90" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C90" s="16"/>
       <c r="D90" s="16"/>
@@ -6963,10 +6936,7 @@
       <c r="F90" s="16"/>
       <c r="G90" s="16"/>
       <c r="H90" s="16"/>
-      <c r="I90" s="16" t="str">
-        <f aca="false">IF(G90="","x","")</f>
-        <v>x</v>
-      </c>
+      <c r="I90" s="16"/>
       <c r="J90" s="16" t="str">
         <f aca="false">IF(H90="","x","")</f>
         <v>x</v>
@@ -6999,7 +6969,7 @@
       </c>
       <c r="T90" s="1" t="str">
         <f aca="false">IF(I90&lt;&gt;"",$B90&amp;"|","")</f>
-        <v>sq ft|</v>
+        <v/>
       </c>
       <c r="U90" s="1" t="str">
         <f aca="false">IF(J90&lt;&gt;"",$B90&amp;"|","")</f>
@@ -7016,10 +6986,10 @@
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B91" s="17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C91" s="16"/>
       <c r="D91" s="16"/>
@@ -7027,10 +6997,7 @@
       <c r="F91" s="16"/>
       <c r="G91" s="16"/>
       <c r="H91" s="16"/>
-      <c r="I91" s="16" t="str">
-        <f aca="false">IF(G91="","x","")</f>
-        <v>x</v>
-      </c>
+      <c r="I91" s="16"/>
       <c r="J91" s="16" t="str">
         <f aca="false">IF(H91="","x","")</f>
         <v>x</v>
@@ -7063,7 +7030,7 @@
       </c>
       <c r="T91" s="1" t="str">
         <f aca="false">IF(I91&lt;&gt;"",$B91&amp;"|","")</f>
-        <v>sq in|</v>
+        <v/>
       </c>
       <c r="U91" s="1" t="str">
         <f aca="false">IF(J91&lt;&gt;"",$B91&amp;"|","")</f>
@@ -7080,10 +7047,10 @@
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B92" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C92" s="16"/>
       <c r="D92" s="16"/>
@@ -7091,10 +7058,7 @@
       <c r="F92" s="16"/>
       <c r="G92" s="16"/>
       <c r="H92" s="16"/>
-      <c r="I92" s="16" t="str">
-        <f aca="false">IF(G92="","x","")</f>
-        <v>x</v>
-      </c>
+      <c r="I92" s="16"/>
       <c r="J92" s="16" t="str">
         <f aca="false">IF(H92="","x","")</f>
         <v>x</v>
@@ -7127,7 +7091,7 @@
       </c>
       <c r="T92" s="1" t="str">
         <f aca="false">IF(I92&lt;&gt;"",$B92&amp;"|","")</f>
-        <v>sq mile|</v>
+        <v/>
       </c>
       <c r="U92" s="1" t="str">
         <f aca="false">IF(J92&lt;&gt;"",$B92&amp;"|","")</f>
@@ -7144,10 +7108,10 @@
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B93" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C93" s="16"/>
       <c r="D93" s="16"/>
@@ -7155,10 +7119,7 @@
       <c r="F93" s="16"/>
       <c r="G93" s="16"/>
       <c r="H93" s="16"/>
-      <c r="I93" s="16" t="str">
-        <f aca="false">IF(G93="","x","")</f>
-        <v>x</v>
-      </c>
+      <c r="I93" s="16"/>
       <c r="J93" s="16" t="str">
         <f aca="false">IF(H93="","x","")</f>
         <v>x</v>
@@ -7191,7 +7152,7 @@
       </c>
       <c r="T93" s="1" t="str">
         <f aca="false">IF(I93&lt;&gt;"",$B93&amp;"|","")</f>
-        <v>sq yd|</v>
+        <v/>
       </c>
       <c r="U93" s="1" t="str">
         <f aca="false">IF(J93&lt;&gt;"",$B93&amp;"|","")</f>
@@ -7208,24 +7169,24 @@
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B94" s="17" t="s">
         <v>180</v>
-      </c>
-      <c r="B94" s="17" t="s">
-        <v>181</v>
       </c>
       <c r="C94" s="16"/>
       <c r="D94" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E94" s="16"/>
       <c r="F94" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G94" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H94" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I94" s="16" t="str">
         <f aca="false">IF(G94="","x","")</f>
@@ -7277,10 +7238,10 @@
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="B95" s="17" t="s">
         <v>182</v>
-      </c>
-      <c r="B95" s="17" t="s">
-        <v>183</v>
       </c>
       <c r="C95" s="16"/>
       <c r="D95" s="16"/>
@@ -7338,24 +7299,24 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="B96" s="17" t="s">
         <v>184</v>
-      </c>
-      <c r="B96" s="17" t="s">
-        <v>185</v>
       </c>
       <c r="C96" s="16"/>
       <c r="D96" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E96" s="16"/>
       <c r="F96" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G96" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H96" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I96" s="16" t="str">
         <f aca="false">IF(G96="","x","")</f>
@@ -7407,10 +7368,10 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="B97" s="17" t="s">
         <v>186</v>
-      </c>
-      <c r="B97" s="17" t="s">
-        <v>187</v>
       </c>
       <c r="C97" s="16"/>
       <c r="D97" s="16"/>
@@ -7468,24 +7429,24 @@
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="B98" s="17" t="s">
         <v>188</v>
-      </c>
-      <c r="B98" s="17" t="s">
-        <v>189</v>
       </c>
       <c r="C98" s="16"/>
       <c r="D98" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E98" s="16"/>
       <c r="F98" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G98" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H98" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I98" s="16" t="str">
         <f aca="false">IF(G98="","x","")</f>
@@ -7537,18 +7498,18 @@
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="B99" s="17" t="s">
         <v>190</v>
-      </c>
-      <c r="B99" s="17" t="s">
-        <v>191</v>
       </c>
       <c r="C99" s="16"/>
       <c r="D99" s="16"/>
       <c r="E99" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F99" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G99" s="16"/>
       <c r="H99" s="16"/>
@@ -7602,10 +7563,10 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="B100" s="17" t="s">
         <v>192</v>
-      </c>
-      <c r="B100" s="17" t="s">
-        <v>193</v>
       </c>
       <c r="C100" s="16"/>
       <c r="D100" s="16"/>
@@ -7663,10 +7624,10 @@
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="B101" s="17" t="s">
         <v>194</v>
-      </c>
-      <c r="B101" s="17" t="s">
-        <v>195</v>
       </c>
       <c r="C101" s="16"/>
       <c r="D101" s="16"/>
@@ -7724,24 +7685,24 @@
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B102" s="17" t="s">
         <v>196</v>
-      </c>
-      <c r="B102" s="17" t="s">
-        <v>197</v>
       </c>
       <c r="C102" s="16"/>
       <c r="D102" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E102" s="16"/>
       <c r="F102" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G102" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H102" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I102" s="16" t="str">
         <f aca="false">IF(G102="","x","")</f>
@@ -7793,16 +7754,16 @@
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B103" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="E103" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F103" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G103" s="16"/>
       <c r="I103" s="16" t="str">
@@ -7852,10 +7813,10 @@
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="F104" s="16"/>
       <c r="G104" s="16"/>
@@ -7906,24 +7867,24 @@
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="B105" s="17" t="s">
         <v>202</v>
-      </c>
-      <c r="B105" s="17" t="s">
-        <v>203</v>
       </c>
       <c r="C105" s="16"/>
       <c r="D105" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E105" s="16"/>
       <c r="F105" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G105" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H105" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I105" s="16" t="str">
         <f aca="false">IF(G105="","x","")</f>
@@ -7975,24 +7936,24 @@
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="B106" s="17" t="s">
         <v>204</v>
-      </c>
-      <c r="B106" s="17" t="s">
-        <v>205</v>
       </c>
       <c r="C106" s="16"/>
       <c r="D106" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E106" s="16"/>
       <c r="F106" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G106" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H106" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I106" s="16" t="str">
         <f aca="false">IF(G106="","x","")</f>
@@ -8044,16 +8005,16 @@
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B107" s="2" t="s">
-        <v>207</v>
-      </c>
       <c r="E107" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F107" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G107" s="16"/>
       <c r="I107" s="16" t="str">
@@ -8103,10 +8064,10 @@
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="B108" s="17" t="s">
         <v>208</v>
-      </c>
-      <c r="B108" s="17" t="s">
-        <v>209</v>
       </c>
       <c r="C108" s="16"/>
       <c r="D108" s="16"/>
@@ -8164,10 +8125,10 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="B109" s="17" t="s">
         <v>210</v>
-      </c>
-      <c r="B109" s="17" t="s">
-        <v>211</v>
       </c>
       <c r="C109" s="16"/>
       <c r="D109" s="16"/>
@@ -8225,10 +8186,10 @@
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="B110" s="17" t="s">
         <v>212</v>
-      </c>
-      <c r="B110" s="17" t="s">
-        <v>213</v>
       </c>
       <c r="C110" s="16"/>
       <c r="D110" s="16"/>
@@ -8286,10 +8247,10 @@
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="B111" s="17" t="s">
         <v>214</v>
-      </c>
-      <c r="B111" s="17" t="s">
-        <v>215</v>
       </c>
       <c r="C111" s="16"/>
       <c r="D111" s="16"/>
@@ -8347,24 +8308,24 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="B112" s="17" t="s">
         <v>216</v>
-      </c>
-      <c r="B112" s="17" t="s">
-        <v>217</v>
       </c>
       <c r="C112" s="16"/>
       <c r="D112" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E112" s="16"/>
       <c r="F112" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G112" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H112" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I112" s="16" t="str">
         <f aca="false">IF(G112="","x","")</f>

</xml_diff>